<commit_message>
- do func TatToan CongNo TGT
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Teamplate_TheNap.xlsx
+++ b/banhang24/Template/ExportExcel/Teamplate_TheNap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>DANH SÁCH THẺ NẠP</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>Ngày lập phiếu</t>
+  </si>
+  <si>
+    <t>Giá trị tất toán</t>
+  </si>
+  <si>
+    <t>Còn nợ</t>
   </si>
 </sst>
 </file>
@@ -205,7 +211,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -300,6 +306,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -585,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,32 +613,36 @@
     <col min="9" max="9" width="17.28515625" style="20" customWidth="1"/>
     <col min="10" max="10" width="17" style="20" customWidth="1"/>
     <col min="11" max="11" width="16.140625" style="20" customWidth="1"/>
-    <col min="12" max="12" width="21.7109375" style="20" customWidth="1"/>
-    <col min="13" max="13" width="19.7109375" style="12" customWidth="1"/>
-    <col min="14" max="15" width="19.7109375" style="11" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="12" width="18.7109375" style="20" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" style="20" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" style="20" customWidth="1"/>
+    <col min="15" max="15" width="19.7109375" style="12" customWidth="1"/>
+    <col min="16" max="17" width="19.7109375" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-    </row>
-    <row r="4" spans="1:15" s="16" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+    </row>
+    <row r="4" spans="1:17" s="16" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -666,17 +679,23 @@
       <c r="L4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -689,11 +708,13 @@
       <c r="J5" s="19"/>
       <c r="K5" s="19"/>
       <c r="L5" s="19"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -706,11 +727,13 @@
       <c r="J6" s="19"/>
       <c r="K6" s="19"/>
       <c r="L6" s="19"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -723,11 +746,13 @@
       <c r="J7" s="19"/>
       <c r="K7" s="19"/>
       <c r="L7" s="19"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -740,11 +765,13 @@
       <c r="J8" s="19"/>
       <c r="K8" s="19"/>
       <c r="L8" s="19"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -757,11 +784,13 @@
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
       <c r="L9" s="19"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -774,11 +803,13 @@
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -791,11 +822,13 @@
       <c r="J11" s="19"/>
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -808,11 +841,13 @@
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
       <c r="L12" s="19"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -825,11 +860,13 @@
       <c r="J13" s="19"/>
       <c r="K13" s="19"/>
       <c r="L13" s="19"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -842,11 +879,13 @@
       <c r="J14" s="19"/>
       <c r="K14" s="19"/>
       <c r="L14" s="19"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -859,11 +898,13 @@
       <c r="J15" s="19"/>
       <c r="K15" s="19"/>
       <c r="L15" s="19"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -876,11 +917,13 @@
       <c r="J16" s="19"/>
       <c r="K16" s="19"/>
       <c r="L16" s="19"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -893,11 +936,13 @@
       <c r="J17" s="19"/>
       <c r="K17" s="19"/>
       <c r="L17" s="19"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -910,11 +955,13 @@
       <c r="J18" s="19"/>
       <c r="K18" s="19"/>
       <c r="L18" s="19"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -927,11 +974,13 @@
       <c r="J19" s="19"/>
       <c r="K19" s="19"/>
       <c r="L19" s="19"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -944,11 +993,13 @@
       <c r="J20" s="19"/>
       <c r="K20" s="19"/>
       <c r="L20" s="19"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -961,11 +1012,13 @@
       <c r="J21" s="19"/>
       <c r="K21" s="19"/>
       <c r="L21" s="19"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -978,11 +1031,13 @@
       <c r="J22" s="19"/>
       <c r="K22" s="19"/>
       <c r="L22" s="19"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -995,11 +1050,13 @@
       <c r="J23" s="19"/>
       <c r="K23" s="19"/>
       <c r="L23" s="19"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -1012,11 +1069,13 @@
       <c r="J24" s="19"/>
       <c r="K24" s="19"/>
       <c r="L24" s="19"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -1029,11 +1088,13 @@
       <c r="J25" s="19"/>
       <c r="K25" s="19"/>
       <c r="L25" s="19"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -1046,11 +1107,13 @@
       <c r="J26" s="19"/>
       <c r="K26" s="19"/>
       <c r="L26" s="19"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -1063,11 +1126,13 @@
       <c r="J27" s="19"/>
       <c r="K27" s="19"/>
       <c r="L27" s="19"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
       <c r="B28" s="23"/>
       <c r="C28" s="23"/>
@@ -1080,11 +1145,13 @@
       <c r="J28" s="25"/>
       <c r="K28" s="25"/>
       <c r="L28" s="25"/>
-      <c r="M28" s="26"/>
-      <c r="N28" s="27"/>
-      <c r="O28" s="27"/>
-    </row>
-    <row r="29" spans="1:15" s="21" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M28" s="25"/>
+      <c r="N28" s="25"/>
+      <c r="O28" s="26"/>
+      <c r="P28" s="27"/>
+      <c r="Q28" s="27"/>
+    </row>
+    <row r="29" spans="1:17" s="21" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
         <v>11</v>
       </c>
@@ -1120,9 +1187,17 @@
         <f xml:space="preserve"> SUM(L$5:L28)</f>
         <v>0</v>
       </c>
-      <c r="M29" s="32"/>
-      <c r="N29" s="30"/>
-      <c r="O29" s="30"/>
+      <c r="M29" s="31">
+        <f xml:space="preserve"> SUM(M$5:M28)</f>
+        <v>0</v>
+      </c>
+      <c r="N29" s="31">
+        <f xml:space="preserve"> SUM(N$5:N28)</f>
+        <v>0</v>
+      </c>
+      <c r="O29" s="32"/>
+      <c r="P29" s="30"/>
+      <c r="Q29" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>